<commit_message>
small fixes + profile_processor add
</commit_message>
<xml_diff>
--- a/test_arr_63.xlsx
+++ b/test_arr_63.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Englishman\Projects\Python\Novatel_data_parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815454E8-22CA-4868-8694-2E05DE775854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA2B836-763B-4E26-AF62-A3DF26800AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="780" windowWidth="18585" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="270" windowWidth="23475" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10443,7 +10443,7 @@
   <dimension ref="A1:J886"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>